<commit_message>
Listados del 7 de agosto de 2024
</commit_message>
<xml_diff>
--- a/Agosto/07 agosto/region sierra/PLANTILLA LISTA DE ASPIRANTES_TECNOLOGICO DE LA SIERRA EXAMEN DE ADMISION ESPECIAL.xlsx
+++ b/Agosto/07 agosto/region sierra/PLANTILLA LISTA DE ASPIRANTES_TECNOLOGICO DE LA SIERRA EXAMEN DE ADMISION ESPECIAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sierra\OneDrive\Escritorio\DEPARTAMENTO DE CIENCIAS BASICAS\PLANTILLA DE ASPIRANTES PARA EXAMEN DE ADMISION ITSS 2023\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\07 agosto\region sierra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F34D6E0-6D52-447E-B171-2CB24916A2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4122FB-5D82-4B9D-82C8-2F1C3455792E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUATEC" sheetId="1" r:id="rId1"/>
@@ -1108,7 +1108,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1145,7 +1145,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1157,13 +1156,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="h:mm\ AM/PM"/>
     </dxf>
@@ -1209,22 +1221,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:M79" totalsRowShown="0">
   <autoFilter ref="A1:M79" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M79">
-    <sortCondition ref="A2:A79"/>
+    <sortCondition ref="E1:E79"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FICHA"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE ASPIRANTE"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CURP"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CORREO ELECTRONICO"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CLAVE CARRERA" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CLAVE CARRERA" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CARRERA"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="VERSION" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FECHA SIMULACRO" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="HORA DE SIMULACRO" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="AULA" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="VERSION" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FECHA SIMULACRO" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="HORA DE SIMULACRO" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="AULA" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1529,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="77" workbookViewId="0">
-      <selection activeCell="N68" sqref="N68"/>
+    <sheetView tabSelected="1" topLeftCell="D50" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="77" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1592,25 +1604,25 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>66</v>
+      <c r="A2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
+        <v>148</v>
+      </c>
+      <c r="D2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="10"/>
@@ -1624,28 +1636,28 @@
       <c r="L2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="9"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>68</v>
+      <c r="A3" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
+        <v>298</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="10"/>
@@ -1659,28 +1671,28 @@
       <c r="L3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>70</v>
+      <c r="A4" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+        <v>299</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="10"/>
@@ -1697,25 +1709,25 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>250</v>
+      <c r="A5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>252</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+        <v>196</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="10"/>
@@ -1730,27 +1742,27 @@
         <v>14</v>
       </c>
       <c r="M5" s="3"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
-        <v>256</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
+        <v>248</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>13</v>
@@ -1770,22 +1782,22 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
+        <v>235</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>13</v>
@@ -1804,23 +1816,23 @@
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
+        <v>127</v>
+      </c>
+      <c r="D8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F8" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>13</v>
@@ -1840,22 +1852,22 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
+        <v>216</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>13</v>
@@ -1875,22 +1887,22 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>249</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
+        <v>227</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>13</v>
@@ -1910,22 +1922,22 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
+        <v>306</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>13</v>
@@ -1945,28 +1957,28 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>81</v>
+        <v>300</v>
+      </c>
+      <c r="B12" t="s">
+        <v>301</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
+        <v>304</v>
+      </c>
+      <c r="D12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18"/>
       <c r="J12" s="15">
         <v>45511</v>
       </c>
@@ -1976,32 +1988,32 @@
       <c r="L12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="3"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>83</v>
+        <v>302</v>
+      </c>
+      <c r="B13" t="s">
+        <v>303</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
+        <v>305</v>
+      </c>
+      <c r="D13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="6"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
       <c r="J13" s="15">
         <v>45511</v>
       </c>
@@ -2011,26 +2023,26 @@
       <c r="L13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="3"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>85</v>
+      <c r="A14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>13</v>
@@ -2049,29 +2061,29 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>258</v>
+      <c r="A15" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>259</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>266</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="15">
         <v>45511</v>
       </c>
@@ -2081,32 +2093,32 @@
       <c r="L15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="20"/>
+      <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>260</v>
+      <c r="A16" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>267</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="15">
         <v>45511</v>
       </c>
@@ -2116,32 +2128,32 @@
       <c r="L16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M16" s="20"/>
+      <c r="M16" s="3"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>262</v>
+      <c r="A17" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>268</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="19"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="6"/>
       <c r="J17" s="15">
         <v>45511</v>
       </c>
@@ -2151,32 +2163,32 @@
       <c r="L17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="20"/>
+      <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>264</v>
+      <c r="A18" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>269</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="19"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="15">
         <v>45511</v>
       </c>
@@ -2186,26 +2198,26 @@
       <c r="L18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M18" s="20"/>
+      <c r="M18" s="3"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>274</v>
+        <v>197</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>13</v>
@@ -2224,20 +2236,23 @@
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>232</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>111</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>209</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>13</v>
@@ -2256,23 +2271,23 @@
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>224</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s">
-        <v>275</v>
+        <v>112</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>210</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>13</v>
@@ -2291,23 +2306,23 @@
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>276</v>
+        <v>198</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>13</v>
@@ -2326,23 +2341,23 @@
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>207</v>
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>277</v>
-      </c>
-      <c r="D23" t="s">
-        <v>208</v>
+        <v>114</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>229</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>13</v>
@@ -2358,26 +2373,26 @@
       <c r="L23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M23" s="20"/>
+      <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="D24" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>13</v>
@@ -2396,23 +2411,23 @@
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>40</v>
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>195</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>13</v>
@@ -2431,29 +2446,29 @@
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="B26" t="s">
-        <v>188</v>
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
-        <v>189</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>48</v>
+        <v>194</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19"/>
+        <v>13</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="6"/>
       <c r="J26" s="15">
         <v>45511</v>
       </c>
@@ -2463,32 +2478,32 @@
       <c r="L26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="20"/>
+      <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="B27" t="s">
-        <v>202</v>
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>203</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>204</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>48</v>
+        <v>292</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
       </c>
       <c r="F27" t="s">
-        <v>205</v>
+        <v>119</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="19"/>
+        <v>13</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="15">
         <v>45511</v>
       </c>
@@ -2498,32 +2513,32 @@
       <c r="L27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M27" s="20"/>
+      <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>212</v>
+      <c r="A28" t="s">
+        <v>293</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>294</v>
       </c>
       <c r="C28" t="s">
-        <v>215</v>
+        <v>295</v>
       </c>
       <c r="D28" t="s">
-        <v>214</v>
+        <v>296</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F28" t="s">
-        <v>205</v>
+        <v>119</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H28" s="18"/>
-      <c r="I28" s="19"/>
+        <v>13</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
       <c r="J28" s="15">
         <v>45511</v>
       </c>
@@ -2533,32 +2548,32 @@
       <c r="L28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M28" s="20"/>
+      <c r="M28" s="19"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="B29" t="s">
-        <v>219</v>
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>220</v>
-      </c>
-      <c r="D29" t="s">
-        <v>221</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>48</v>
+        <v>71</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>205</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="19"/>
+        <v>16</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="6"/>
       <c r="J29" s="15">
         <v>45511</v>
       </c>
@@ -2568,32 +2583,32 @@
       <c r="L29" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M29" s="20"/>
+      <c r="M29" s="9"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>237</v>
-      </c>
-      <c r="B30" t="s">
-        <v>240</v>
+        <v>67</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>241</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>48</v>
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>223</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>205</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H30" s="18"/>
-      <c r="I30" s="19"/>
+        <v>16</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="6"/>
       <c r="J30" s="15">
         <v>45511</v>
       </c>
@@ -2603,32 +2618,32 @@
       <c r="L30" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M30" s="20"/>
+      <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>238</v>
-      </c>
-      <c r="B31" t="s">
-        <v>242</v>
+        <v>69</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>48</v>
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>205</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
+        <v>16</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="6"/>
       <c r="J31" s="15">
         <v>45511</v>
       </c>
@@ -2638,102 +2653,99 @@
       <c r="L31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M31" s="20"/>
+      <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>239</v>
-      </c>
-      <c r="B32" t="s">
-        <v>244</v>
+        <v>253</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>250</v>
       </c>
       <c r="C32" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="D32" t="s">
-        <v>285</v>
-      </c>
-      <c r="E32" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="15">
+        <v>45511</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="3"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>274</v>
+      </c>
+      <c r="E33" t="s">
         <v>48</v>
       </c>
-      <c r="F32" t="s">
-        <v>205</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="15">
-        <v>45511</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M32" s="20"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>279</v>
-      </c>
-      <c r="B33" t="s">
-        <v>280</v>
-      </c>
-      <c r="C33" t="s">
-        <v>283</v>
-      </c>
-      <c r="D33" t="s">
-        <v>286</v>
-      </c>
-      <c r="E33" s="12" t="s">
+      <c r="F33" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="15">
+        <v>45511</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="3"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
         <v>48</v>
       </c>
-      <c r="F33" t="s">
-        <v>205</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H33" s="18"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="15">
-        <v>45511</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M33" s="20"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>281</v>
-      </c>
-      <c r="B34" t="s">
-        <v>282</v>
-      </c>
-      <c r="C34" t="s">
-        <v>284</v>
-      </c>
-      <c r="D34" t="s">
-        <v>287</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>48</v>
-      </c>
       <c r="F34" t="s">
-        <v>205</v>
+        <v>93</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H34" s="18"/>
-      <c r="I34" s="19"/>
+        <v>13</v>
+      </c>
+      <c r="H34" s="10"/>
+      <c r="I34" s="6"/>
       <c r="J34" s="15">
         <v>45511</v>
       </c>
@@ -2743,26 +2755,26 @@
       <c r="L34" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M34" s="20"/>
+      <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F35" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>13</v>
@@ -2782,22 +2794,22 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="E36" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F36" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>13</v>
@@ -2817,22 +2829,22 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>207</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>277</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="E37" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F37" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>13</v>
@@ -2848,26 +2860,26 @@
       <c r="L37" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M37" s="3"/>
+      <c r="M37" s="19"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F38" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>13</v>
@@ -2887,22 +2899,22 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>236</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F39" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>13</v>
@@ -2921,29 +2933,29 @@
       <c r="M39" s="3"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>95</v>
+      <c r="A40" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B40" t="s">
+        <v>188</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="D40" t="s">
-        <v>197</v>
-      </c>
-      <c r="E40" t="s">
-        <v>64</v>
+        <v>189</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F40" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H40" s="17"/>
+      <c r="I40" s="18"/>
       <c r="J40" s="15">
         <v>45511</v>
       </c>
@@ -2953,32 +2965,32 @@
       <c r="L40" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M40" s="3"/>
+      <c r="M40" s="19"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>232</v>
+      <c r="A41" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>202</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="E41" t="s">
-        <v>64</v>
+        <v>203</v>
+      </c>
+      <c r="D41" t="s">
+        <v>204</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F41" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="10"/>
-      <c r="I41" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H41" s="17"/>
+      <c r="I41" s="18"/>
       <c r="J41" s="15">
         <v>45511</v>
       </c>
@@ -2988,32 +3000,32 @@
       <c r="L41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M41" s="3"/>
+      <c r="M41" s="19"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>224</v>
+      <c r="A42" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" t="s">
+        <v>213</v>
       </c>
       <c r="C42" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="E42" t="s">
-        <v>64</v>
+        <v>215</v>
+      </c>
+      <c r="D42" t="s">
+        <v>214</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F42" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="10"/>
-      <c r="I42" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H42" s="17"/>
+      <c r="I42" s="18"/>
       <c r="J42" s="15">
         <v>45511</v>
       </c>
@@ -3023,32 +3035,32 @@
       <c r="L42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M42" s="3"/>
+      <c r="M42" s="19"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>99</v>
+      <c r="A43" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" t="s">
+        <v>219</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>220</v>
       </c>
       <c r="D43" t="s">
-        <v>198</v>
-      </c>
-      <c r="E43" t="s">
-        <v>64</v>
+        <v>221</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F43" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H43" s="17"/>
+      <c r="I43" s="18"/>
       <c r="J43" s="15">
         <v>45511</v>
       </c>
@@ -3058,32 +3070,32 @@
       <c r="L43" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M43" s="3"/>
+      <c r="M43" s="19"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>101</v>
+        <v>237</v>
+      </c>
+      <c r="B44" t="s">
+        <v>240</v>
       </c>
       <c r="C44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="E44" t="s">
-        <v>64</v>
+        <v>241</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F44" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="10"/>
-      <c r="I44" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H44" s="17"/>
+      <c r="I44" s="18"/>
       <c r="J44" s="15">
         <v>45511</v>
       </c>
@@ -3093,32 +3105,32 @@
       <c r="L44" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M44" s="3"/>
+      <c r="M44" s="19"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>102</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>103</v>
+        <v>238</v>
+      </c>
+      <c r="B45" t="s">
+        <v>242</v>
       </c>
       <c r="C45" t="s">
-        <v>115</v>
-      </c>
-      <c r="D45" t="s">
-        <v>291</v>
-      </c>
-      <c r="E45" t="s">
-        <v>64</v>
+        <v>243</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F45" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H45" s="10"/>
-      <c r="I45" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H45" s="17"/>
+      <c r="I45" s="18"/>
       <c r="J45" s="15">
         <v>45511</v>
       </c>
@@ -3128,32 +3140,32 @@
       <c r="L45" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M45" s="3"/>
+      <c r="M45" s="19"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>105</v>
+        <v>239</v>
+      </c>
+      <c r="B46" t="s">
+        <v>244</v>
       </c>
       <c r="C46" t="s">
-        <v>116</v>
+        <v>245</v>
       </c>
       <c r="D46" t="s">
-        <v>195</v>
-      </c>
-      <c r="E46" t="s">
-        <v>64</v>
+        <v>285</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F46" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H46" s="10"/>
-      <c r="I46" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H46" s="17"/>
+      <c r="I46" s="18"/>
       <c r="J46" s="15">
         <v>45511</v>
       </c>
@@ -3163,32 +3175,32 @@
       <c r="L46" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M46" s="3"/>
+      <c r="M46" s="19"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>107</v>
+        <v>279</v>
+      </c>
+      <c r="B47" t="s">
+        <v>280</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>283</v>
       </c>
       <c r="D47" t="s">
-        <v>194</v>
-      </c>
-      <c r="E47" t="s">
-        <v>64</v>
+        <v>286</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F47" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="10"/>
-      <c r="I47" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
       <c r="J47" s="15">
         <v>45511</v>
       </c>
@@ -3198,32 +3210,32 @@
       <c r="L47" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M47" s="3"/>
+      <c r="M47" s="19"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>109</v>
+        <v>281</v>
+      </c>
+      <c r="B48" t="s">
+        <v>282</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>284</v>
       </c>
       <c r="D48" t="s">
-        <v>292</v>
-      </c>
-      <c r="E48" t="s">
-        <v>64</v>
+        <v>287</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="F48" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="10"/>
-      <c r="I48" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="H48" s="17"/>
+      <c r="I48" s="18"/>
       <c r="J48" s="15">
         <v>45511</v>
       </c>
@@ -3233,32 +3245,32 @@
       <c r="L48" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M48" s="3"/>
+      <c r="M48" s="19"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>293</v>
-      </c>
-      <c r="B49" t="s">
-        <v>294</v>
+        <v>179</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="C49" t="s">
-        <v>295</v>
+        <v>181</v>
       </c>
       <c r="D49" t="s">
-        <v>296</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>64</v>
+        <v>225</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>186</v>
       </c>
       <c r="F49" t="s">
-        <v>119</v>
+        <v>182</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="18"/>
-      <c r="I49" s="19"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="6"/>
       <c r="J49" s="15">
         <v>45511</v>
       </c>
@@ -3268,26 +3280,26 @@
       <c r="L49" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M49" s="20"/>
+      <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>148</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>297</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>184</v>
+        <v>256</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>13</v>
@@ -3307,22 +3319,22 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>22</v>
       </c>
       <c r="D51" t="s">
-        <v>298</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>184</v>
+        <v>23</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>13</v>
@@ -3342,22 +3354,22 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" t="s">
-        <v>299</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>184</v>
+        <v>26</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>13</v>
@@ -3376,23 +3388,23 @@
       <c r="M52" s="3"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B53" t="s">
-        <v>138</v>
+      <c r="A53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="C53" t="s">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
-        <v>196</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>184</v>
+        <v>206</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>13</v>
@@ -3411,23 +3423,23 @@
       <c r="M53" s="3"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B54" t="s">
-        <v>135</v>
+      <c r="A54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="D54" t="s">
-        <v>248</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>184</v>
+        <v>249</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>13</v>
@@ -3446,23 +3458,23 @@
       <c r="M54" s="3"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B55" t="s">
-        <v>132</v>
+      <c r="A55" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>235</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>184</v>
+        <v>187</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>13</v>
@@ -3482,22 +3494,22 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" t="s">
-        <v>234</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>184</v>
+        <v>89</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>13</v>
@@ -3517,22 +3529,22 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>217</v>
+        <v>83</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
-      </c>
-      <c r="D57" t="s">
-        <v>216</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>184</v>
+        <v>90</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>13</v>
@@ -3552,22 +3564,22 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D58" t="s">
-        <v>227</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>184</v>
+        <v>257</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F58" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>13</v>
@@ -3587,28 +3599,28 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>125</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>126</v>
+        <v>258</v>
+      </c>
+      <c r="B59" t="s">
+        <v>259</v>
       </c>
       <c r="C59" t="s">
-        <v>130</v>
+        <v>266</v>
       </c>
       <c r="D59" t="s">
-        <v>306</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>184</v>
+        <v>270</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F59" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H59" s="10"/>
-      <c r="I59" s="6"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="18"/>
       <c r="J59" s="15">
         <v>45511</v>
       </c>
@@ -3618,32 +3630,32 @@
       <c r="L59" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M59" s="3"/>
+      <c r="M59" s="19"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="B60" t="s">
-        <v>301</v>
+        <v>261</v>
       </c>
       <c r="C60" t="s">
-        <v>304</v>
+        <v>267</v>
       </c>
       <c r="D60" t="s">
-        <v>307</v>
-      </c>
-      <c r="E60" s="16" t="s">
-        <v>184</v>
+        <v>271</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F60" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H60" s="18"/>
-      <c r="I60" s="19"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="18"/>
       <c r="J60" s="15">
         <v>45511</v>
       </c>
@@ -3653,32 +3665,32 @@
       <c r="L60" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M60" s="20"/>
+      <c r="M60" s="19"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>263</v>
       </c>
       <c r="C61" t="s">
-        <v>305</v>
+        <v>268</v>
       </c>
       <c r="D61" t="s">
-        <v>308</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>184</v>
+        <v>272</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F61" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H61" s="18"/>
-      <c r="I61" s="19"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="18"/>
       <c r="J61" s="15">
         <v>45511</v>
       </c>
@@ -3688,32 +3700,32 @@
       <c r="L61" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M61" s="20"/>
+      <c r="M61" s="19"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
-        <v>149</v>
+      <c r="A62" t="s">
+        <v>264</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>265</v>
       </c>
       <c r="C62" t="s">
-        <v>151</v>
+        <v>269</v>
       </c>
       <c r="D62" t="s">
-        <v>193</v>
-      </c>
-      <c r="E62" s="17" t="s">
-        <v>185</v>
+        <v>273</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="F62" t="s">
-        <v>177</v>
+        <v>92</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H62" s="10"/>
-      <c r="I62" s="6"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="18"/>
       <c r="J62" s="15">
         <v>45511</v>
       </c>
@@ -3723,22 +3735,22 @@
       <c r="L62" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M62" s="3"/>
+      <c r="M62" s="19"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>192</v>
-      </c>
-      <c r="E63" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="E63" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F63" t="s">
@@ -3762,15 +3774,18 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B64" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
-      </c>
-      <c r="E64" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D64" t="s">
+        <v>192</v>
+      </c>
+      <c r="E64" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F64" t="s">
@@ -3794,18 +3809,15 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B65" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
-      </c>
-      <c r="D65" t="s">
-        <v>309</v>
-      </c>
-      <c r="E65" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E65" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F65" t="s">
@@ -3828,19 +3840,19 @@
       <c r="M65" s="3"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>166</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>161</v>
+      <c r="A66" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" t="s">
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D66" t="s">
-        <v>231</v>
-      </c>
-      <c r="E66" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="E66" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F66" t="s">
@@ -3864,18 +3876,18 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>211</v>
-      </c>
-      <c r="E67" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="E67" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F67" t="s">
@@ -3899,22 +3911,22 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C68" t="s">
-        <v>173</v>
-      </c>
-      <c r="D68" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="E68" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D68" t="s">
+        <v>211</v>
+      </c>
+      <c r="E68" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F68" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>13</v>
@@ -3934,22 +3946,22 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C69" t="s">
-        <v>174</v>
-      </c>
-      <c r="D69" t="s">
-        <v>222</v>
-      </c>
-      <c r="E69" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="E69" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>13</v>
@@ -3969,18 +3981,18 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C70" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D70" t="s">
-        <v>310</v>
-      </c>
-      <c r="E70" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E70" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F70" t="s">
@@ -4004,18 +4016,18 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>311</v>
-      </c>
-      <c r="B71" t="s">
-        <v>312</v>
+        <v>170</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>165</v>
       </c>
       <c r="C71" t="s">
-        <v>317</v>
+        <v>175</v>
       </c>
       <c r="D71" t="s">
-        <v>318</v>
-      </c>
-      <c r="E71" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="E71" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F71" t="s">
@@ -4024,8 +4036,8 @@
       <c r="G71" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H71" s="18"/>
-      <c r="I71" s="19"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="6"/>
       <c r="J71" s="15">
         <v>45511</v>
       </c>
@@ -4035,22 +4047,22 @@
       <c r="L71" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M71" s="20"/>
+      <c r="M71" s="3"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B72" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C72" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D72" t="s">
-        <v>320</v>
-      </c>
-      <c r="E72" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="E72" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F72" t="s">
@@ -4059,8 +4071,8 @@
       <c r="G72" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H72" s="18"/>
-      <c r="I72" s="19"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="18"/>
       <c r="J72" s="15">
         <v>45511</v>
       </c>
@@ -4070,22 +4082,22 @@
       <c r="L72" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M72" s="20"/>
+      <c r="M72" s="19"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B73" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C73" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D73" t="s">
-        <v>322</v>
-      </c>
-      <c r="E73" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>185</v>
       </c>
       <c r="F73" t="s">
@@ -4094,8 +4106,8 @@
       <c r="G73" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H73" s="18"/>
-      <c r="I73" s="19"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="18"/>
       <c r="J73" s="15">
         <v>45511</v>
       </c>
@@ -4105,32 +4117,32 @@
       <c r="L73" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M73" s="20"/>
+      <c r="M73" s="19"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>179</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>180</v>
+        <v>315</v>
+      </c>
+      <c r="B74" t="s">
+        <v>316</v>
       </c>
       <c r="C74" t="s">
-        <v>181</v>
+        <v>321</v>
       </c>
       <c r="D74" t="s">
-        <v>225</v>
-      </c>
-      <c r="E74" s="17" t="s">
-        <v>186</v>
+        <v>322</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="F74" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H74" s="10"/>
-      <c r="I74" s="6"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="18"/>
       <c r="J74" s="15">
         <v>45511</v>
       </c>
@@ -4140,7 +4152,7 @@
       <c r="L74" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M74" s="3"/>
+      <c r="M74" s="19"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B75" s="11"/>
@@ -4202,17 +4214,20 @@
     <mergeCell ref="N5:O5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D42" r:id="rId1" xr:uid="{254DFF46-03C8-4FA8-9D82-FA75396BBABF}"/>
-    <hyperlink ref="D13" r:id="rId2" xr:uid="{81F13EEA-B0C2-487E-9062-6FF812992CF1}"/>
-    <hyperlink ref="D44" r:id="rId3" xr:uid="{5B519905-CDD2-411A-9724-2981E33CD340}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{298F0159-94D0-4401-9D24-129787FC9F5E}"/>
-    <hyperlink ref="D41" r:id="rId5" xr:uid="{60B9BFF2-C31C-425F-9850-599A6BDD1005}"/>
-    <hyperlink ref="D2" r:id="rId6" xr:uid="{E368E712-D11E-4155-9392-1F2B81B95EEC}"/>
-    <hyperlink ref="D30" r:id="rId7" xr:uid="{DE1FB1ED-92F3-4CEA-AB71-279F31834E01}"/>
-    <hyperlink ref="D31" r:id="rId8" xr:uid="{97A85631-1088-4F66-9DAB-6F0B0FDD6CB4}"/>
-    <hyperlink ref="D12" r:id="rId9" xr:uid="{D87E42C1-F550-46B5-8E26-4069F0D16E8F}"/>
-    <hyperlink ref="D68" r:id="rId10" xr:uid="{35DDA148-C123-44CB-8557-C3CB9A1F1E9B}"/>
+    <hyperlink ref="D21" r:id="rId1" xr:uid="{254DFF46-03C8-4FA8-9D82-FA75396BBABF}"/>
+    <hyperlink ref="D57" r:id="rId2" xr:uid="{81F13EEA-B0C2-487E-9062-6FF812992CF1}"/>
+    <hyperlink ref="D23" r:id="rId3" xr:uid="{5B519905-CDD2-411A-9724-2981E33CD340}"/>
+    <hyperlink ref="D52" r:id="rId4" xr:uid="{298F0159-94D0-4401-9D24-129787FC9F5E}"/>
+    <hyperlink ref="D20" r:id="rId5" xr:uid="{60B9BFF2-C31C-425F-9850-599A6BDD1005}"/>
+    <hyperlink ref="D29" r:id="rId6" xr:uid="{E368E712-D11E-4155-9392-1F2B81B95EEC}"/>
+    <hyperlink ref="D44" r:id="rId7" xr:uid="{DE1FB1ED-92F3-4CEA-AB71-279F31834E01}"/>
+    <hyperlink ref="D45" r:id="rId8" xr:uid="{97A85631-1088-4F66-9DAB-6F0B0FDD6CB4}"/>
+    <hyperlink ref="D56" r:id="rId9" xr:uid="{D87E42C1-F550-46B5-8E26-4069F0D16E8F}"/>
+    <hyperlink ref="D69" r:id="rId10" xr:uid="{35DDA148-C123-44CB-8557-C3CB9A1F1E9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId11"/>

</xml_diff>